<commit_message>
Implementation of the taskbar sheet
</commit_message>
<xml_diff>
--- a/系统占用内存分布.xlsx
+++ b/系统占用内存分布.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mayx-my.sharepoint.com/personal/kalinote_say-huahuo_com/Documents/Projects/OSProject/KalinoteOS/KalinoteOS1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="11_AD4DA82427541F7ACA7EB89E404D00AC6BE8DE13" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7E3B4C92-B40C-4DE1-B082-9F3921DB1991}"/>
+  <xr:revisionPtr revIDLastSave="603" documentId="11_AD4DA82427541F7ACA7EB89E404D00AC6BE8DE13" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1B1226FB-E697-4780-BA0E-12F2E5A357DE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>注9：0x00400000以后的内存会在系统启动进入保护模式检查内存后清空，所以如果要保存系统数据，需要在清空后保存</t>
+    <t>注9：0x00400000以后的内存会在系统启动进入保护模式检查内存后清空，在0x400000以前的内存不会被应用程序使用，作为系统内存</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -588,7 +588,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,11 +608,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,35 +650,8 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -949,7 +952,7 @@
   <dimension ref="A1:V100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -962,67 +965,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="12" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8"/>
-      <c r="B3" s="13"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
@@ -1033,50 +1036,50 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="18"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
       <c r="J4" s="8"/>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="13"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1087,50 +1090,50 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="18" t="s">
+      <c r="K5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="18"/>
-      <c r="U5" s="18"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="8"/>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
-      <c r="B7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="8" t="s">
         <v>5</v>
       </c>
@@ -1141,50 +1144,50 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="18" t="s">
+      <c r="K7" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
     </row>
     <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
-      <c r="B9" s="13"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1195,32 +1198,32 @@
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
     </row>
     <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="8"/>
       <c r="K10" s="5" t="s">
         <v>61</v>
@@ -1229,26 +1232,26 @@
         <v>64</v>
       </c>
       <c r="M10" s="8"/>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="7"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="8" t="s">
         <v>66</v>
       </c>
       <c r="Q10" s="8"/>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7" t="s">
+      <c r="S10" s="10"/>
+      <c r="T10" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="7"/>
+      <c r="U10" s="10"/>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
-      <c r="B11" s="13"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1266,28 +1269,28 @@
         <v>65</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="7" t="s">
+      <c r="N11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O11" s="7"/>
+      <c r="O11" s="10"/>
       <c r="P11" s="8" t="s">
         <v>67</v>
       </c>
       <c r="Q11" s="8"/>
-      <c r="R11" s="7" t="s">
+      <c r="R11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7" t="s">
+      <c r="S11" s="10"/>
+      <c r="T11" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="U11" s="7"/>
+      <c r="U11" s="10"/>
     </row>
     <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="13"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1308,7 +1311,7 @@
       <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1329,136 +1332,147 @@
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="18" t="s">
+      <c r="K14" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="18"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
     </row>
     <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
       <c r="J15" s="8"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
     </row>
     <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="19" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="8" t="s">
@@ -1476,7 +1490,7 @@
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="8" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1504,7 @@
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8"/>
-      <c r="B24" s="16"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="8" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1520,7 @@
       <c r="A25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -1522,7 +1536,7 @@
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8"/>
-      <c r="B26" s="20"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="8" t="s">
         <v>14</v>
       </c>
@@ -1536,7 +1550,7 @@
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8"/>
-      <c r="B27" s="20"/>
+      <c r="B27" s="7"/>
       <c r="C27" s="8" t="s">
         <v>18</v>
       </c>
@@ -1552,7 +1566,7 @@
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="20"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
@@ -1566,7 +1580,7 @@
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="20"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
@@ -1580,7 +1594,7 @@
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="20"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
@@ -1596,26 +1610,26 @@
       <c r="A31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="17" t="s">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="12" t="s">
+      <c r="B32" s="20"/>
+      <c r="C32" s="11" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="8"/>
@@ -1624,13 +1638,13 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="17"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="10"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -1638,11 +1652,11 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="17"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="8" t="s">
         <v>42</v>
       </c>
@@ -1652,11 +1666,11 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="17"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="8" t="s">
         <v>43</v>
       </c>
@@ -1666,27 +1680,27 @@
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="17"/>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="12" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="17"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="18"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="10"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="8" t="s">
         <v>54</v>
       </c>
@@ -1696,13 +1710,13 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
-      <c r="J37" s="17"/>
+      <c r="J37" s="18"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="10"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="8" t="s">
         <v>74</v>
       </c>
@@ -1712,11 +1726,11 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
-      <c r="J38" s="17"/>
+      <c r="J38" s="18"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="B39" s="10"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
@@ -1724,7 +1738,7 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
-      <c r="J39" s="17"/>
+      <c r="J39" s="18"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1789,35 +1803,14 @@
     <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="K9:U9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="K14:U14"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="K6:U6"/>
-    <mergeCell ref="K7:U7"/>
-    <mergeCell ref="K8:U8"/>
-    <mergeCell ref="C32:I33"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="K5:U5"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C14:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C27:I29"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:I39"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="A33:A36"/>
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="J2:J30"/>
     <mergeCell ref="C31:I31"/>
@@ -1834,22 +1827,43 @@
     <mergeCell ref="J31:J39"/>
     <mergeCell ref="K3:U3"/>
     <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C32:I33"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="K5:U5"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C14:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C27:I29"/>
     <mergeCell ref="R11:S11"/>
     <mergeCell ref="T10:U10"/>
     <mergeCell ref="T11:U11"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C38:I39"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="C11:I13"/>
+    <mergeCell ref="K4:U4"/>
+    <mergeCell ref="K14:U15"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="K6:U6"/>
+    <mergeCell ref="K7:U7"/>
+    <mergeCell ref="K8:U8"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A2:A11"/>
-    <mergeCell ref="C11:I13"/>
     <mergeCell ref="K2:U2"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="K4:U4"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="K9:U9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L13:M13"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>